<commit_message>
update step 3 and some data extraction files
</commit_message>
<xml_diff>
--- a/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Binch.xlsx
+++ b/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Binch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wageningenur4-my.sharepoint.com/personal/esther_beukhof_wur_nl/Documents/Projects/SEAwise/SEAwise GitHub/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{364C45A6-2E05-4AC3-8A64-FC7E53566F10}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5E6BA9B5-45FC-444A-801C-D2951C0D5FF1}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{4025E7B6-130C-49E7-B057-CC7B29E6FA5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{924119D6-8177-4577-8AC1-A24C7F8588DE}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2388,7 +2388,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2863" uniqueCount="724">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2861" uniqueCount="724">
   <si>
     <t>SearchID</t>
   </si>
@@ -5593,9 +5593,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CI77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="AC8" sqref="AC8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5723,7 +5723,7 @@
       <c r="CH1" s="13"/>
       <c r="CI1" s="13"/>
     </row>
-    <row r="2" spans="1:87" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:87" s="12" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>68</v>
       </c>
@@ -16163,8 +16163,8 @@
       </c>
       <c r="AD65" s="20"/>
       <c r="AE65" s="20"/>
-      <c r="AF65" s="20" t="s">
-        <v>374</v>
+      <c r="AF65" s="20">
+        <v>4.2</v>
       </c>
       <c r="AG65" s="20" t="s">
         <v>111</v>
@@ -16334,8 +16334,8 @@
       </c>
       <c r="AD66" s="20"/>
       <c r="AE66" s="20"/>
-      <c r="AF66" s="20" t="s">
-        <v>374</v>
+      <c r="AF66" s="20">
+        <v>4.2</v>
       </c>
       <c r="AG66" s="20" t="s">
         <v>111</v>
@@ -20381,21 +20381,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006AB0F5ECCA53DA47AEBDEAEE6167985F" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="abe771af6212f3f785694fa6f4ad1686">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -20509,17 +20494,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{296C6747-B437-4BFD-90D3-AF1F913D3FA0}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -20533,17 +20534,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{296C6747-B437-4BFD-90D3-AF1F913D3FA0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
final changes data extraction files and Step1 run for report
</commit_message>
<xml_diff>
--- a/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Binch.xlsx
+++ b/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_Binch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wageningenur4-my.sharepoint.com/personal/esther_beukhof_wur_nl/Documents/Projects/SEAwise/SEAwise GitHub/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{4025E7B6-130C-49E7-B057-CC7B29E6FA5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{924119D6-8177-4577-8AC1-A24C7F8588DE}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{55AAF37A-66B8-4EE0-B65A-BD216287DE1D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FAC6D289-B042-4DE5-A972-B546C4F6EFCE}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-3495" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataExtraction" sheetId="1" r:id="rId1"/>
@@ -2388,7 +2388,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2861" uniqueCount="724">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2861" uniqueCount="725">
   <si>
     <t>SearchID</t>
   </si>
@@ -5043,6 +5043,9 @@
   </si>
   <si>
     <t>Clutch size _ Egg size _ Hatching success</t>
+  </si>
+  <si>
+    <t>Observations of attachment</t>
   </si>
 </sst>
 </file>
@@ -5593,9 +5596,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CI77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AL1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC8" sqref="AC8"/>
+      <selection pane="bottomLeft" activeCell="AM8" sqref="AM8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10018,7 +10021,7 @@
       <c r="AS27" s="20"/>
       <c r="AT27" s="20"/>
       <c r="AU27" s="20" t="s">
-        <v>707</v>
+        <v>724</v>
       </c>
       <c r="AV27" s="20" t="s">
         <v>113</v>
@@ -18277,7 +18280,7 @@
     <mergeCell ref="AM1:AP1"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI17 AI3:AJ16 P3:Q37 AI18:AJ1048576 AN3:AN1048576 AR3:AS1048576" xr:uid="{147CE50E-8A31-47FF-849B-125EEE18B3C2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI17 AI3:AJ16 P3:Q37 AR3:AS1048576 AN3:AN1048576 AI18:AJ1048576" xr:uid="{147CE50E-8A31-47FF-849B-125EEE18B3C2}">
       <formula1>INDIRECT(O3)</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK17" xr:uid="{97164204-0BAF-4351-AC4A-2A40314A5C36}">
@@ -20381,6 +20384,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006AB0F5ECCA53DA47AEBDEAEE6167985F" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="abe771af6212f3f785694fa6f4ad1686">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -20494,15 +20506,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -20510,6 +20513,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{296C6747-B437-4BFD-90D3-AF1F913D3FA0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20525,25 +20536,17 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>